<commit_message>
"Get Info Product To Excel"
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/GetProducts.xlsx
+++ b/src/test/resources/excelData/GetProducts.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FinalProjectAutoTest\cms-user-checkout-testing\src\test\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3890A76-7C4B-4FB4-B2C6-93F2D66841CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA6E2EC-B7CF-426E-8C43-475BE59D641B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FDDAB713-9CAE-4FC5-9D33-067753119640}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="InfoProduct" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,15 +35,166 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="42">
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>DiscountPrice</t>
+  </si>
+  <si>
+    <t>Laptop Asus</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Aqua</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Laptop asus vừa mạnh vừa đẹp</t>
+  </si>
+  <si>
+    <t>https://cms.anhtester.com/public/uploads/all/lBlf5f6r8uudgHJomw8hKYSCruMgPwpIAzKpojIH.webp</t>
+  </si>
+  <si>
+    <t>https://cms.anhtester.com/product/laptop-asus-7</t>
+  </si>
+  <si>
+    <t>18/08/2025 10:56</t>
+  </si>
+  <si>
+    <t>Laptop Gaming</t>
+  </si>
+  <si>
+    <t>$1,000.00</t>
+  </si>
+  <si>
+    <t>/pc</t>
+  </si>
+  <si>
+    <t>$900.00</t>
+  </si>
+  <si>
+    <t>Crimson, Red</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Đồ công nghệ cao</t>
+  </si>
+  <si>
+    <t>https://cms.anhtester.com/public/uploads/all/krVAUGG4HQdU3RDel4dlgNfBTl4YvN7nB6GsSLxv.png</t>
+  </si>
+  <si>
+    <t>https://cms.anhtester.com/product/laptop-gaming</t>
+  </si>
+  <si>
+    <t>18/08/2025 10:57</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:06</t>
+  </si>
+  <si>
+    <t>$3,000.00</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:17</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:29</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:34</t>
+  </si>
+  <si>
+    <t>/PC</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:39</t>
+  </si>
+  <si>
+    <t>$1,000.00 /pc</t>
+  </si>
+  <si>
+    <t>18/08/2025 11:40</t>
+  </si>
+  <si>
+    <t>18/08/2025 22:55</t>
+  </si>
+  <si>
+    <t>Product_Name</t>
+  </si>
+  <si>
+    <t>Available_Quantity</t>
+  </si>
+  <si>
+    <t>Image_URL</t>
+  </si>
+  <si>
+    <t>Product_URL</t>
+  </si>
+  <si>
+    <t>Captured_Time</t>
+  </si>
+  <si>
+    <t>19/08/2025 00:09</t>
+  </si>
+  <si>
+    <t>19/08/2025 00:10</t>
+  </si>
+  <si>
+    <t>19/08/2025 00:20</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF6AAB73"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +213,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +574,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12DE2CD-4C88-40B5-988F-C8AE2EC6E965}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.6015625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.8125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.40625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.00390625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.90625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.1015625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.4140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="81.5625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="39.890625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.9140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>